<commit_message>
"Updated .DS_Store and Monitoring ST.xlsx files in public directory"
</commit_message>
<xml_diff>
--- a/public/templates/Monitoring ST.xlsx
+++ b/public/templates/Monitoring ST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Laravel Project/SiAPP Transda v2/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EED4846-E666-A64A-BD93-A0BB077FD056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4075715B-6661-2346-BE91-6F90104B8134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="16760" xr2:uid="{D8B18E26-9386-0943-A948-FD67555A8AC8}"/>
   </bookViews>
@@ -278,23 +278,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -312,6 +312,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -372,106 +412,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -810,8 +750,8 @@
   </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="E40" sqref="E7:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -841,36 +781,36 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -885,7 +825,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
@@ -1209,7 +1149,7 @@
       <c r="C32" s="6"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="10"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -1221,7 +1161,7 @@
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="8"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
@@ -1325,18 +1265,18 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="D7:D40">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:G31 E34:G40 F33:G33 E7:F7 E32 G32">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+  <conditionalFormatting sqref="E7:F7 E8:G31 E32 G32 F33:G33 E34:G40">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThanOrEqual">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
"Added Pelaporan model to ExportController, updated ExportController to include Pelaporan data in export, and modified Monitoring ST.xlsx template."
</commit_message>
<xml_diff>
--- a/public/templates/Monitoring ST.xlsx
+++ b/public/templates/Monitoring ST.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Laravel Project/SiAPP Transda v2/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842276BB-FE38-F845-AF55-B41A022EB486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7B8335-4616-C140-AD80-12E4E80C25D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>PEMANTAUAN SURAT TUGAS</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>Perwakilan BPKP Provinsi Kalimantan Utara</t>
+  </si>
+  <si>
+    <t>Jumlah Upload Laporan</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -426,16 +459,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -470,336 +493,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
@@ -1141,37 +834,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="7" width="14" customWidth="1"/>
-    <col min="8" max="14" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
+    <col min="4" max="11" width="15.83203125" customWidth="1"/>
+    <col min="12" max="14" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
@@ -1187,8 +882,14 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1204,8 +905,20 @@
       <c r="G6" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1227,8 +940,20 @@
       <c r="G7" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -1250,8 +975,20 @@
       <c r="G8" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3</v>
+      </c>
+      <c r="K8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>3</v>
       </c>
@@ -1273,8 +1010,20 @@
       <c r="G9" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3</v>
+      </c>
+      <c r="K9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>4</v>
       </c>
@@ -1296,8 +1045,20 @@
       <c r="G10" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3</v>
+      </c>
+      <c r="K10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -1319,8 +1080,20 @@
       <c r="G11" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -1342,8 +1115,20 @@
       <c r="G12" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>7</v>
       </c>
@@ -1365,8 +1150,20 @@
       <c r="G13" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>8</v>
       </c>
@@ -1388,8 +1185,20 @@
       <c r="G14" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>9</v>
       </c>
@@ -1411,8 +1220,20 @@
       <c r="G15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>10</v>
       </c>
@@ -1434,8 +1255,20 @@
       <c r="G16" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>11</v>
       </c>
@@ -1457,8 +1290,20 @@
       <c r="G17" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>12</v>
       </c>
@@ -1480,8 +1325,20 @@
       <c r="G18" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3">
+        <v>3</v>
+      </c>
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>13</v>
       </c>
@@ -1503,8 +1360,20 @@
       <c r="G19" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>14</v>
       </c>
@@ -1526,8 +1395,20 @@
       <c r="G20" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>15</v>
       </c>
@@ -1549,8 +1430,20 @@
       <c r="G21" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>16</v>
       </c>
@@ -1572,8 +1465,20 @@
       <c r="G22" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <v>3</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>17</v>
       </c>
@@ -1595,8 +1500,20 @@
       <c r="G23" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>3</v>
+      </c>
+      <c r="J23" s="3">
+        <v>3</v>
+      </c>
+      <c r="K23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>18</v>
       </c>
@@ -1618,8 +1535,20 @@
       <c r="G24" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>2</v>
+      </c>
+      <c r="J24" s="3">
+        <v>2</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>19</v>
       </c>
@@ -1641,8 +1570,20 @@
       <c r="G25" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
+      <c r="I25" s="3">
+        <v>3</v>
+      </c>
+      <c r="J25" s="3">
+        <v>3</v>
+      </c>
+      <c r="K25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>20</v>
       </c>
@@ -1664,8 +1605,20 @@
       <c r="G26" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+      <c r="I26" s="3">
+        <v>3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>3</v>
+      </c>
+      <c r="K26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>21</v>
       </c>
@@ -1687,8 +1640,20 @@
       <c r="G27" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" s="3">
+        <v>2</v>
+      </c>
+      <c r="I27" s="3">
+        <v>3</v>
+      </c>
+      <c r="J27" s="3">
+        <v>3</v>
+      </c>
+      <c r="K27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>22</v>
       </c>
@@ -1710,8 +1675,20 @@
       <c r="G28" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="3">
+        <v>2</v>
+      </c>
+      <c r="I28" s="3">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3">
+        <v>3</v>
+      </c>
+      <c r="K28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>23</v>
       </c>
@@ -1733,8 +1710,20 @@
       <c r="G29" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>3</v>
+      </c>
+      <c r="J29" s="3">
+        <v>3</v>
+      </c>
+      <c r="K29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>24</v>
       </c>
@@ -1756,8 +1745,20 @@
       <c r="G30" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>3</v>
+      </c>
+      <c r="J30" s="3">
+        <v>3</v>
+      </c>
+      <c r="K30" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>25</v>
       </c>
@@ -1779,8 +1780,20 @@
       <c r="G31" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>3</v>
+      </c>
+      <c r="J31" s="3">
+        <v>2</v>
+      </c>
+      <c r="K31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>26</v>
       </c>
@@ -1802,8 +1815,20 @@
       <c r="G32" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H32" s="3">
+        <v>2</v>
+      </c>
+      <c r="I32" s="3">
+        <v>3</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>27</v>
       </c>
@@ -1825,8 +1850,20 @@
       <c r="G33" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2</v>
+      </c>
+      <c r="K33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>28</v>
       </c>
@@ -1848,8 +1885,20 @@
       <c r="G34" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H34" s="3">
+        <v>3</v>
+      </c>
+      <c r="I34" s="3">
+        <v>3</v>
+      </c>
+      <c r="J34" s="3">
+        <v>3</v>
+      </c>
+      <c r="K34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>29</v>
       </c>
@@ -1871,8 +1920,20 @@
       <c r="G35" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3">
+        <v>3</v>
+      </c>
+      <c r="J35" s="3">
+        <v>3</v>
+      </c>
+      <c r="K35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>30</v>
       </c>
@@ -1894,8 +1955,20 @@
       <c r="G36" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>3</v>
+      </c>
+      <c r="J36" s="3">
+        <v>3</v>
+      </c>
+      <c r="K36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>31</v>
       </c>
@@ -1917,8 +1990,20 @@
       <c r="G37" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+      <c r="I37" s="3">
+        <v>3</v>
+      </c>
+      <c r="J37" s="3">
+        <v>3</v>
+      </c>
+      <c r="K37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>32</v>
       </c>
@@ -1940,8 +2025,20 @@
       <c r="G38" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>3</v>
+      </c>
+      <c r="J38" s="3">
+        <v>3</v>
+      </c>
+      <c r="K38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>33</v>
       </c>
@@ -1963,8 +2060,20 @@
       <c r="G39" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+      <c r="I39" s="3">
+        <v>3</v>
+      </c>
+      <c r="J39" s="3">
+        <v>3</v>
+      </c>
+      <c r="K39" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>34</v>
       </c>
@@ -1986,39 +2095,76 @@
       <c r="G40" s="3">
         <v>3</v>
       </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+      <c r="I40" s="3">
+        <v>3</v>
+      </c>
+      <c r="J40" s="3">
+        <v>3</v>
+      </c>
+      <c r="K40" s="3">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D40">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:G14 E7:F7 E34:G40 F33:G33 E32 G32 E16:G31">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="E7:F7 E8:G14 E16:G31 E32 G32 F33:G33 E34:G40">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G15">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>1</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:H40">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:J7 I8:K14 I16:K31 I32 K32 J33:K33 I34:K40">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:K15">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="59" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>